<commit_message>
changed hardcoded methods into general methods for init and exit
</commit_message>
<xml_diff>
--- a/ICS4U7 IA - Data Porter/bin/farms4life2016/init/hardcode these jobs.xlsx
+++ b/ICS4U7 IA - Data Porter/bin/farms4life2016/init/hardcode these jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yucen\Computer_IA\data file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Evacuation\Gr 12\ICS bundles\Git Stuff\VSCode\ICS4U7 IA - Data Porter\src\farms4life2016\init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0007CAF6-9F1C-432A-9E88-20419967EA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26092D1E-ACCA-4144-AE39-F65C2A7318BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BF396AB3-64EB-4875-8BE6-C7817A640FFF}"/>
+    <workbookView xWindow="5265" yWindow="2565" windowWidth="23940" windowHeight="14025" xr2:uid="{BF396AB3-64EB-4875-8BE6-C7817A640FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,17 +457,17 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -507,7 +507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -524,7 +524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -541,7 +541,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -558,7 +558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -575,7 +575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -592,7 +592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -612,7 +612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -629,7 +629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -646,7 +646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -663,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -680,7 +680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
added date support for jobs.
</commit_message>
<xml_diff>
--- a/ICS4U7 IA - Data Porter/bin/farms4life2016/init/hardcode these jobs.xlsx
+++ b/ICS4U7 IA - Data Porter/bin/farms4life2016/init/hardcode these jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Evacuation\Gr 12\ICS bundles\Git Stuff\VSCode\ICS4U7 IA - Data Porter\src\farms4life2016\init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26092D1E-ACCA-4144-AE39-F65C2A7318BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040316E-F67B-485F-BDC6-99A520511AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="2565" windowWidth="23940" windowHeight="14025" xr2:uid="{BF396AB3-64EB-4875-8BE6-C7817A640FFF}"/>
+    <workbookView xWindow="8925" yWindow="2955" windowWidth="23940" windowHeight="14025" xr2:uid="{BF396AB3-64EB-4875-8BE6-C7817A640FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>E_BOM.xml</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Feb 29, 2004 (00:00:00 EST)</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,16 +478,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -492,16 +501,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>15</v>
@@ -512,16 +524,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -529,16 +544,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -546,16 +564,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -563,33 +584,39 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -597,16 +624,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -617,16 +647,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,16 +667,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
         <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -651,16 +687,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,16 +707,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -685,16 +727,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>